<commit_message>
excel unit test insert_notification
</commit_message>
<xml_diff>
--- a/server/tests/data/excel/create_sheet_test_data.xlsx
+++ b/server/tests/data/excel/create_sheet_test_data.xlsx
@@ -3,27 +3,33 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="test-data" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="test-result" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +40,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -44,14 +57,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,7 +158,7 @@
     <tableColumn id="6" name="ColumnDescription"/>
     <tableColumn id="7" name="ExpectedResult"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -149,10 +167,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -190,71 +208,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -282,7 +300,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -305,11 +323,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -318,13 +336,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -334,7 +352,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -343,7 +361,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -352,7 +370,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -360,10 +378,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -435,260 +453,261 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15.08984375" customWidth="1" min="1" max="1"/>
-    <col width="13.54296875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="16.90625" customWidth="1" min="3" max="3"/>
-    <col width="14.1796875" customWidth="1" min="4" max="4"/>
-    <col width="13.54296875" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="18.7265625" customWidth="1" min="6" max="6"/>
-    <col width="15.453125" customWidth="1" min="7" max="7"/>
+    <col width="15.14785714285714" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
+    <col width="16.86214285714286" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
+    <col width="14.14785714285714" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
+    <col width="18.71928571428571" bestFit="1" customWidth="1" style="3" min="6" max="6"/>
+    <col width="15.43357142857143" bestFit="1" customWidth="1" style="3" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>TestCaseName</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>SheetName</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>SheetDescription</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>ColumnName</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>ColumnType</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>ColumnDescription</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>ExpectedResult</t>
         </is>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Valid_Sheet_String_Column</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Bảng sản phẩm</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Thông tin về sản phẩm</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>product_name</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>Tên sản phẩm</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Empty_Sheet_Name</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="B3" s="3" t="n"/>
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Thông tin về sản phẩm</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>product_name</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>Tên sản phẩm</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Empty_Sheet_Description</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Bảng sản phẩm</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n"/>
-      <c r="D4" t="inlineStr">
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>product_name</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>Tên sản phẩm</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>Empty_Column_Name</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Bảng sản phẩm</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>Thông tin về sản phẩm</t>
         </is>
       </c>
-      <c r="D5" s="2" t="n"/>
-      <c r="E5" t="inlineStr">
+      <c r="D5" s="3" t="n"/>
+      <c r="E5" s="3" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="3" t="inlineStr">
         <is>
           <t>Tên sản phẩm</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>Invalid_Column_Type</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>Bảng sản phẩm</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>Thông tin về sản phẩm</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>product_name</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="3" t="inlineStr">
         <is>
           <t>Float</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="3" t="inlineStr">
         <is>
           <t>Tên sản phẩm</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="7" ht="18.75" customHeight="1">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>Empty_Column_Description</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>Bảng sản phẩm</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>Thông tin về sản phẩm</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>product_name</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="3" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="F7" s="2" t="n"/>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="F7" s="3" t="n"/>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
     </row>
@@ -708,70 +727,77 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.54296875" bestFit="1" customWidth="1" min="1" max="8"/>
-    <col width="13.54296875" bestFit="1" customWidth="1" style="1" min="9" max="9"/>
-    <col width="13.54296875" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="8" max="8"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="9" max="9"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>TestCaseName</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>SheetName</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>SheetDescription</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>ColumnName</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>ColumnType</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>ColumnDescription</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>ExpectedResult</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>ActualResult</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Log</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="18.75" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
           <t>Valid_Sheet_String_Column</t>
@@ -804,21 +830,21 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>True</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2025-06-07 11:45:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
+          <t>2025-06-07 11:58:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
           <t>Empty_Sheet_Name</t>
@@ -846,12 +872,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>False</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>False</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -861,11 +887,11 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2025-06-07 11:45:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
+          <t>2025-06-07 11:58:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
       <c r="A4" t="inlineStr">
         <is>
           <t>Empty_Sheet_Description</t>
@@ -893,12 +919,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>False</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>False</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -908,11 +934,11 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2025-06-07 11:45:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
+          <t>2025-06-07 11:58:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="58.5" customHeight="1">
       <c r="A5" t="inlineStr">
         <is>
           <t>Empty_Column_Name</t>
@@ -940,12 +966,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>False</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>False</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -958,11 +984,11 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2025-06-07 11:45:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
+          <t>2025-06-07 11:58:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="58.5" customHeight="1">
       <c r="A6" t="inlineStr">
         <is>
           <t>Invalid_Column_Type</t>
@@ -995,12 +1021,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>False</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>False</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -1013,11 +1039,11 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2025-06-07 11:45:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
+          <t>2025-06-07 11:58:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="58.5" customHeight="1">
       <c r="A7" t="inlineStr">
         <is>
           <t>Empty_Column_Description</t>
@@ -1045,12 +1071,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>False</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>False</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1063,12 +1089,11 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2025-06-07 11:45:37</t>
+          <t>2025-06-07 11:58:44</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
excel unit test insert_script, insert_interest
</commit_message>
<xml_diff>
--- a/server/tests/data/excel/create_sheet_test_data.xlsx
+++ b/server/tests/data/excel/create_sheet_test_data.xlsx
@@ -840,7 +840,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2025-06-07 11:58:44</t>
+          <t>2025-06-07 13:13:38</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2025-06-07 11:58:44</t>
+          <t>2025-06-07 13:13:38</t>
         </is>
       </c>
     </row>
@@ -934,7 +934,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2025-06-07 11:58:44</t>
+          <t>2025-06-07 13:13:38</t>
         </is>
       </c>
     </row>
@@ -984,7 +984,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2025-06-07 11:58:44</t>
+          <t>2025-06-07 13:13:38</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2025-06-07 11:58:44</t>
+          <t>2025-06-07 13:13:38</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2025-06-07 11:58:44</t>
+          <t>2025-06-07 13:13:38</t>
         </is>
       </c>
     </row>

</xml_diff>